<commit_message>
Fix links for Chris Hardwick - first ones seen with post_id
</commit_message>
<xml_diff>
--- a/data/2020-06-30/SCW Weekly Comp 2020-06-30 (Responses).xlsx
+++ b/data/2020-06-30/SCW Weekly Comp 2020-06-30 (Responses).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2020-06-30\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BE4141-34E8-41F4-B9AC-1EF7FAC7B217}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BACF30A8-3EEA-4DB1-BCB1-EEE8550525B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="4740" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -1484,14 +1484,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:CY110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V85" sqref="V85"/>
+      <selection pane="bottomLeft" activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1499,7 +1499,7 @@
     <col min="1" max="109" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44012.667063819448</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>9.5500000000000007</v>
       </c>
     </row>
-    <row r="3" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44012.698465138892</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>9.52</v>
       </c>
     </row>
-    <row r="4" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44012.699659965278</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44012.701098344907</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>21.63</v>
       </c>
     </row>
-    <row r="6" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44012.753220057872</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44012.873967233798</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>19.68</v>
       </c>
     </row>
-    <row r="8" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44012.884377326394</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44012.933587824074</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>33.71</v>
       </c>
     </row>
-    <row r="10" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44012.938628101852</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44012.93929844907</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44012.941634988427</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>10.49</v>
       </c>
     </row>
-    <row r="13" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44012.942901550923</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44013.062393229164</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>18.36</v>
       </c>
     </row>
-    <row r="15" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44013.203973506941</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>44013.467577164352</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>10.96</v>
       </c>
     </row>
-    <row r="17" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>44013.612784594909</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>44013.665975370372</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>44013.68748310185</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>24.27</v>
       </c>
     </row>
-    <row r="20" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44013.737888530093</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>44013.742012777773</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>18.04</v>
       </c>
     </row>
-    <row r="22" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>44013.742973587963</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>48.29</v>
       </c>
     </row>
-    <row r="23" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>44013.757055787035</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>44013.863801064814</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>9.7899999999999991</v>
       </c>
     </row>
-    <row r="25" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>44013.86464255787</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>6.83</v>
       </c>
     </row>
-    <row r="26" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>44013.865466354167</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>5.46</v>
       </c>
     </row>
-    <row r="27" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>44013.866260011579</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>13.44</v>
       </c>
     </row>
-    <row r="28" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>44014.254071238422</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>44014.452275416668</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>44014.564502800931</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>44014.63299643519</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>19.07</v>
       </c>
     </row>
-    <row r="32" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>44014.642738206021</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>44014.654069108801</v>
       </c>
@@ -3068,7 +3068,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>44014.757927754632</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="35" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>44014.925825451384</v>
       </c>
@@ -3150,7 +3150,7 @@
         <v>53.79</v>
       </c>
     </row>
-    <row r="36" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>44014.926660682875</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>44014.946201087965</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="38" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>44015.808549467591</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="39" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>44015.811079016203</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="40" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>44015.831227465278</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="41" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>44015.851829120365</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="42" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>44016.24086953704</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>44016.254513958338</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>41.2</v>
       </c>
     </row>
-    <row r="44" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>44016.261909768524</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44016.287522824074</v>
       </c>
@@ -3548,7 +3548,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>44016.566202025468</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>15.93</v>
       </c>
     </row>
-    <row r="47" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>44016.567039560185</v>
       </c>
@@ -3636,7 +3636,7 @@
         <v>36.53</v>
       </c>
     </row>
-    <row r="48" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>44016.568158368056</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>18.75</v>
       </c>
     </row>
-    <row r="49" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>44016.569029375001</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>40.19</v>
       </c>
     </row>
-    <row r="50" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>44016.569661990739</v>
       </c>
@@ -3762,7 +3762,7 @@
         <v>21.43</v>
       </c>
     </row>
-    <row r="51" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>44016.570399143515</v>
       </c>
@@ -3806,7 +3806,7 @@
         <v>11.31</v>
       </c>
     </row>
-    <row r="52" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>44016.572087592591</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>6.16</v>
       </c>
     </row>
-    <row r="53" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>44016.592072951389</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="54" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>44016.647120567126</v>
       </c>
@@ -3929,7 +3929,7 @@
         <v>18.059999999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>44016.649083483797</v>
       </c>
@@ -3970,7 +3970,7 @@
         <v>35.26</v>
       </c>
     </row>
-    <row r="56" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>44016.71805575231</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>19.22</v>
       </c>
     </row>
-    <row r="57" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>44016.719334837966</v>
       </c>
@@ -4052,7 +4052,7 @@
         <v>22.99</v>
       </c>
     </row>
-    <row r="58" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>44016.73149096065</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>44016.803174189816</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="60" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>44016.803533877319</v>
       </c>
@@ -4169,7 +4169,7 @@
         <v>43.19</v>
       </c>
     </row>
-    <row r="61" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>44016.818846354166</v>
       </c>
@@ -4210,7 +4210,7 @@
         <v>19.059999999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>44016.819967129632</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>13.62</v>
       </c>
     </row>
-    <row r="63" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>44016.826340092593</v>
       </c>
@@ -4292,7 +4292,7 @@
         <v>16.52</v>
       </c>
     </row>
-    <row r="64" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:98" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>44016.82789695602</v>
       </c>
@@ -4333,7 +4333,7 @@
         <v>11.42</v>
       </c>
     </row>
-    <row r="65" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>44016.829106203702</v>
       </c>
@@ -4377,7 +4377,7 @@
         <v>30.36</v>
       </c>
     </row>
-    <row r="66" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>44016.830465729166</v>
       </c>
@@ -4421,7 +4421,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="67" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>44016.831758738423</v>
       </c>
@@ -4456,7 +4456,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>44016.835293333337</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>12.82</v>
       </c>
     </row>
-    <row r="69" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>44016.838284282407</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="70" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>44016.839446307873</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="71" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>44016.840676793981</v>
       </c>
@@ -4608,7 +4608,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="72" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>44016.875299328705</v>
       </c>
@@ -4643,7 +4643,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>44017.123144849538</v>
       </c>
@@ -4669,7 +4669,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="74" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>44017.127902060187</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="75" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>44017.399677546295</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>48.2</v>
       </c>
     </row>
-    <row r="76" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>44017.614769629625</v>
       </c>
@@ -4771,7 +4771,7 @@
         <v>11.62</v>
       </c>
     </row>
-    <row r="77" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>44017.915587858792</v>
       </c>
@@ -4809,7 +4809,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="78" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>44017.918150833335</v>
       </c>
@@ -4847,7 +4847,7 @@
         <v>28.71</v>
       </c>
     </row>
-    <row r="79" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>44018.085349201385</v>
       </c>
@@ -4888,7 +4888,7 @@
         <v>11.44</v>
       </c>
     </row>
-    <row r="80" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>44018.086785370368</v>
       </c>
@@ -4929,7 +4929,7 @@
         <v>38.53</v>
       </c>
     </row>
-    <row r="81" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>44018.087754953704</v>
       </c>
@@ -4970,7 +4970,7 @@
         <v>8.4600000000000009</v>
       </c>
     </row>
-    <row r="82" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>44018.089119386575</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>25.95</v>
       </c>
     </row>
-    <row r="83" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>44018.090727719908</v>
       </c>
@@ -5052,7 +5052,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="84" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>44018.092088518519</v>
       </c>
@@ -5093,7 +5093,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="85" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>44018.251381203707</v>
       </c>
@@ -5137,7 +5137,7 @@
         <v>20.51</v>
       </c>
     </row>
-    <row r="86" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>44018.262955266204</v>
       </c>
@@ -5178,7 +5178,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="87" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>44018.264951400459</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="88" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>44018.273906863426</v>
       </c>
@@ -5263,7 +5263,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="89" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>44018.417837152781</v>
       </c>
@@ -5304,7 +5304,7 @@
         <v>44.91</v>
       </c>
     </row>
-    <row r="90" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>44018.454129085643</v>
       </c>
@@ -5339,7 +5339,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="91" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>44018.473640682874</v>
       </c>
@@ -5380,7 +5380,7 @@
         <v>15.44</v>
       </c>
     </row>
-    <row r="92" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>44018.474719710648</v>
       </c>
@@ -5421,7 +5421,7 @@
         <v>34.020000000000003</v>
       </c>
     </row>
-    <row r="93" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>44018.476020694448</v>
       </c>
@@ -5462,7 +5462,7 @@
         <v>7.13</v>
       </c>
     </row>
-    <row r="94" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>44018.477150474537</v>
       </c>
@@ -5497,7 +5497,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="95" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>44018.553152858796</v>
       </c>
@@ -5538,7 +5538,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="96" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>44018.554091597223</v>
       </c>
@@ -5579,7 +5579,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="97" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>44018.820859166663</v>
       </c>
@@ -5620,7 +5620,7 @@
         <v>24.95</v>
       </c>
     </row>
-    <row r="98" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>44018.821913391206</v>
       </c>
@@ -5664,7 +5664,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="99" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>44018.870374421298</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="100" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>44018.871354618052</v>
       </c>
@@ -5743,7 +5743,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="101" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>44018.941588506947</v>
       </c>
@@ -5778,7 +5778,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="102" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>44019.022765057874</v>
       </c>
@@ -5819,7 +5819,7 @@
         <v>8.32</v>
       </c>
     </row>
-    <row r="103" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>44019.023649074079</v>
       </c>
@@ -5860,7 +5860,7 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="104" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>44019.02440436343</v>
       </c>
@@ -5901,7 +5901,7 @@
         <v>22.45</v>
       </c>
     </row>
-    <row r="105" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>44019.025516226851</v>
       </c>
@@ -5942,7 +5942,7 @@
         <v>16.13</v>
       </c>
     </row>
-    <row r="106" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>44019.025820706018</v>
       </c>
@@ -5983,7 +5983,7 @@
         <v>25.41</v>
       </c>
     </row>
-    <row r="107" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>44019.027127615744</v>
       </c>
@@ -6024,7 +6024,7 @@
         <v>17.77</v>
       </c>
     </row>
-    <row r="108" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>44019.403244131943</v>
       </c>
@@ -6047,7 +6047,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="109" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>44019.40422744213</v>
       </c>
@@ -6073,7 +6073,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="110" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>44019.406242743054</v>
       </c>
@@ -6112,13 +6112,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:CY110" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Jason Green"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:CY110" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <customSheetViews>
     <customSheetView guid="{43D299FD-6CE4-4E11-96EB-0BB285424472}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>